<commit_message>
Deleted saponarin in Excel data.
</commit_message>
<xml_diff>
--- a/Data/NEG_Metabolites.xlsx
+++ b/Data/NEG_Metabolites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirozmoreno.1/Documents/GitHub/Urospatha/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4ss0\Documents\Ikiam21062022\U_sagittifolia_tubers\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47232AB-D603-2148-959D-F3549F761467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA95BE-77DF-43CA-A726-10F658BC1911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="20740" windowHeight="11760" xr2:uid="{10CB7462-686D-42CB-A9AA-EF17DF0B17CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{10CB7462-686D-42CB-A9AA-EF17DF0B17CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <t>NCGC00380271-01</t>
   </si>
   <si>
-    <t>Saponarin</t>
-  </si>
-  <si>
     <t>Nictoflorin</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>p-Coumaric acid</t>
+  </si>
+  <si>
+    <t>Vicenin</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -618,17 +618,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B989DFA-4618-49EB-9F18-4BB79616CDF5}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +637,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -650,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -661,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -672,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -683,7 +681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -694,7 +692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -705,7 +703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -716,7 +714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -727,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -738,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -749,7 +747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -760,7 +758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -771,7 +769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -782,7 +780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -793,7 +791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -804,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -815,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -826,18 +824,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -848,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -859,7 +857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -870,7 +868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -881,7 +879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -892,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -903,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -914,7 +912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -925,7 +923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -936,7 +934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -947,7 +945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -958,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -969,7 +967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -980,7 +978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -991,34 +989,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -1041,17 +1039,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="fd700a0b-3029-45a3-b1ab-0b32e8b2ae24" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a59348b-6ef9-45b8-b0fb-04cd720027bf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100776E4A71A5314245913E8264657548C2" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="336726ceb6bc02cf2d0017bf94662676">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0a59348b-6ef9-45b8-b0fb-04cd720027bf" xmlns:ns3="fd700a0b-3029-45a3-b1ab-0b32e8b2ae24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7663cab4eb8d137c0542ce4e06646eae" ns2:_="" ns3:_="">
     <xsd:import namespace="0a59348b-6ef9-45b8-b0fb-04cd720027bf"/>
@@ -1234,6 +1221,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="fd700a0b-3029-45a3-b1ab-0b32e8b2ae24" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a59348b-6ef9-45b8-b0fb-04cd720027bf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA8FC927-01FF-4B1C-B37A-738DA43FC9B1}">
   <ds:schemaRefs>
@@ -1243,17 +1241,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2DFC979-EAAB-4CE6-BB5C-C29C6DC39921}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fd700a0b-3029-45a3-b1ab-0b32e8b2ae24"/>
-    <ds:schemaRef ds:uri="0a59348b-6ef9-45b8-b0fb-04cd720027bf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C737A54-2963-444D-821E-1DE4D136D85A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1270,4 +1257,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2DFC979-EAAB-4CE6-BB5C-C29C6DC39921}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fd700a0b-3029-45a3-b1ab-0b32e8b2ae24"/>
+    <ds:schemaRef ds:uri="0a59348b-6ef9-45b8-b0fb-04cd720027bf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>